<commit_message>
highlight those cells with data validation
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/books/validation.xlsx
+++ b/src/main/webapp/WEB-INF/books/validation.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Documents/workspace/KEIKAI-SPACE/dev-ref/src/main/webapp/WEB-INF/books/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C773CFC2-41B1-CD40-82E8-8CEFC95EB251}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="105" windowWidth="18195" windowHeight="7230"/>
+    <workbookView xWindow="38760" yWindow="3800" windowWidth="21100" windowHeight="12340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="validation" sheetId="1" r:id="rId1"/>
@@ -16,6 +22,30 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Hawk Chen</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{FA5127B8-0365-5E40-BD9A-06D34EF425E4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Those yellow cells contain input validation</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
@@ -55,8 +85,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -88,14 +118,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -189,11 +232,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -203,86 +251,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -294,7 +279,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="C7EDCC"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -329,7 +314,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -361,9 +346,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -395,6 +398,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -570,122 +591,123 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" customWidth="1"/>
+    <col min="3" max="3" width="24.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="6"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="11"/>
     </row>
-    <row r="2" spans="1:4" ht="18.75">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="12" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="14" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18.75">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="12" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="8"/>
+      <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="1:4" ht="18.75">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="13">
         <v>41590</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="18.75">
-      <c r="A5" s="12"/>
+    <row r="5" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A5" s="8"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="8"/>
+      <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:4" ht="18.75">
-      <c r="A6" s="12"/>
+    <row r="6" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A6" s="8"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="8"/>
+      <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:4" ht="18.75">
-      <c r="A7" s="7" t="s">
+    <row r="7" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="8"/>
+      <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="9"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="11"/>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="5"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <dataValidations count="6">
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="Beginning date cannot be a past date" sqref="B4">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="Beginning date cannot be a past date" sqref="B4" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>TODAY()</formula1>
     </dataValidation>
-    <dataValidation type="whole" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Infomation" error="More than 10 days of leave requires special approval." sqref="D4">
+    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Infomation" error="More than 10 days of leave requires special approval." sqref="D4" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>0</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="textLength" errorStyle="warning" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid" error="length should equal to 5" promptTitle="Your ID" prompt="5 characters ID" sqref="D2">
+    <dataValidation type="textLength" errorStyle="warning" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid" error="length should equal to 5" promptTitle="Your ID" prompt="5 characters ID" sqref="D2" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>5</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Unkown Type" error="You should select from drop-down list." sqref="B3">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Unkown Type" error="You should select from drop-down list." sqref="B3" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"Vacation, Sickness, Annual, Military, Maternity"</formula1>
     </dataValidation>
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>0.333333333333333</formula1>
       <formula2>0.75</formula2>
     </dataValidation>
-    <dataValidation type="textLength" errorStyle="information" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Notice" error="Please enter your name" sqref="B2">
+    <dataValidation type="textLength" errorStyle="information" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Notice" error="Please enter your name" sqref="B2" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>2</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>